<commit_message>
minor changes to formatting
</commit_message>
<xml_diff>
--- a/Medium dashboard.xlsx
+++ b/Medium dashboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romandogadin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romandogadin/Documents/GitHub/excel-dashboard-indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37A7351-E96F-1D4D-BCFC-D16E17793D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A39771-BAA8-5940-B39A-B245C5DB0214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="16680" xr2:uid="{4C132304-4FB9-420E-A19E-177B7C24FD04}"/>
   </bookViews>
@@ -23,8 +23,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data FDI'!$A$1:$D$61</definedName>
     <definedName name="_xlchart.v5.0" hidden="1">Dashboard!$B$11</definedName>
     <definedName name="_xlchart.v5.1" hidden="1">Dashboard!$K$2</definedName>
-    <definedName name="_xlchart.v5.2" hidden="1">Dashboard!$B$11</definedName>
-    <definedName name="_xlchart.v5.3" hidden="1">Dashboard!$K$2</definedName>
     <definedName name="Other">'Other Stats'!$B$1:$F$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -130,7 +128,8 @@
     <t>Life Expectancy (years)</t>
   </si>
   <si>
-    <t>Unemployment %</t>
+    <t>Unemployment 
+%</t>
   </si>
 </sst>
 </file>
@@ -251,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -356,21 +355,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -419,6 +403,12 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,13 +424,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1128,11 +1112,11 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v5.3</cx:f>
+        <cx:f>_xlchart.v5.1</cx:f>
       </cx:strDim>
       <cx:numDim type="colorVal">
-        <cx:f>_xlchart.v5.3</cx:f>
-        <cx:nf>_xlchart.v5.2</cx:nf>
+        <cx:f>_xlchart.v5.1</cx:f>
+        <cx:nf>_xlchart.v5.0</cx:nf>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4746,9 +4730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583A65D5-9620-4258-AB73-2FCE46B5A566}">
   <dimension ref="B1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4764,17 +4746,17 @@
       <c r="K1" s="10"/>
     </row>
     <row r="2" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="26" t="str">
         <f>UPPER("Economic Indicators for ") &amp; UPPER(K2)</f>
         <v>ECONOMIC INDICATORS FOR UNITED STATES</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
       <c r="J2" s="11" t="s">
         <v>11</v>
       </c>
@@ -4783,12 +4765,12 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="str">
+      <c r="B4" s="23" t="str">
         <f>"FDI Flow for "&amp;$K$2</f>
         <v>FDI Flow for United States</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
       <c r="K4" s="7" t="s">
         <v>12</v>
       </c>
@@ -4820,7 +4802,7 @@
         <f>INDEX('Data Inflation'!$B$2:$D$7,MATCH(Dashboard!$B6,'Data Inflation'!$A$2:$A$7,0),MATCH(Dashboard!$K$2,'Data Inflation'!$B$1:$D$1,0))</f>
         <v>2.2400000000000002</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="22">
         <f ca="1">OFFSET('Data Interest Rates'!B1,COUNTA('Data Interest Rates'!D:D)-1,MATCH(Dashboard!$K$2,'Data Interest Rates'!B1:D1,0)-1)</f>
         <v>5.08</v>
       </c>
@@ -4837,7 +4819,7 @@
         <f>INDEX('Data Inflation'!$B$2:$D$7,MATCH(Dashboard!$B7,'Data Inflation'!$A$2:$A$7,0),MATCH(Dashboard!$K$2,'Data Inflation'!$B$1:$D$1,0))</f>
         <v>1.8</v>
       </c>
-      <c r="K7" s="20"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
@@ -4886,7 +4868,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K11" s="20">
+      <c r="K11" s="22">
         <f ca="1">OFFSET('Data Inflation'!B1,COUNTA('Data Inflation'!D:D)-1,MATCH(Dashboard!$K$2,'Data Inflation'!B1:D1,0)-1)</f>
         <v>5.8</v>
       </c>
@@ -4902,7 +4884,7 @@
       <c r="D12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="20"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="2:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="18" cm="1">
@@ -4952,7 +4934,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13" style="26" customWidth="1"/>
+    <col min="3" max="3" width="13" style="20" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
@@ -4966,7 +4948,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -4980,7 +4962,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="21">
         <v>32103.508069895001</v>
       </c>
       <c r="D2" t="s">
@@ -5004,7 +4986,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="21">
         <v>9048.9529144990993</v>
       </c>
       <c r="D3" t="s">
@@ -5024,7 +5006,7 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="21">
         <v>2300.9203681473</v>
       </c>
       <c r="D4" t="s">
@@ -5044,7 +5026,7 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="21">
         <v>44364.412431639001</v>
       </c>
       <c r="D5" t="s">
@@ -5058,7 +5040,7 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="21">
         <v>33819</v>
       </c>
       <c r="D6" t="s">
@@ -5072,7 +5054,7 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="21">
         <v>-5428</v>
       </c>
       <c r="D7" t="s">
@@ -5086,7 +5068,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="21">
         <v>107366</v>
       </c>
       <c r="D8" t="s">
@@ -5100,7 +5082,7 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="21">
         <v>80658</v>
       </c>
       <c r="D9" t="s">
@@ -5114,7 +5096,7 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="21">
         <v>5203.3678993424001</v>
       </c>
       <c r="D10" t="s">
@@ -5128,7 +5110,7 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="21">
         <v>2843.6623197038998</v>
       </c>
       <c r="D11" t="s">
@@ -5142,7 +5124,7 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="21">
         <v>1088.7457081361999</v>
       </c>
       <c r="D12" t="s">
@@ -5156,7 +5138,7 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="21">
         <v>1616.4624045481</v>
       </c>
       <c r="D13" t="s">
@@ -5170,7 +5152,7 @@
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="21">
         <v>-11812.149055641001</v>
       </c>
       <c r="D14" t="s">
@@ -5184,7 +5166,7 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="21">
         <v>32487.238386932</v>
       </c>
       <c r="D15" t="s">
@@ -5198,7 +5180,7 @@
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="21">
         <v>30698.060234813998</v>
       </c>
       <c r="D16" t="s">
@@ -5212,7 +5194,7 @@
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="21">
         <v>2534.4563552833001</v>
       </c>
       <c r="D17" t="s">
@@ -5226,7 +5208,7 @@
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="21">
         <v>67787</v>
       </c>
       <c r="D18" t="s">
@@ -5240,7 +5222,7 @@
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="21">
         <v>67918</v>
       </c>
       <c r="D19" t="s">
@@ -5254,7 +5236,7 @@
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="21">
         <v>53827</v>
       </c>
       <c r="D20" t="s">
@@ -5268,7 +5250,7 @@
       <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="21">
         <v>67184</v>
       </c>
       <c r="D21" t="s">
@@ -5282,7 +5264,7 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="21">
         <v>3061.6280064817001</v>
       </c>
       <c r="D22" t="s">
@@ -5296,7 +5278,7 @@
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="21">
         <v>2353.837748682</v>
       </c>
       <c r="D23" t="s">
@@ -5310,7 +5292,7 @@
       <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="21">
         <v>2643.8538582652</v>
       </c>
       <c r="D24" t="s">
@@ -5324,7 +5306,7 @@
       <c r="B25" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="21">
         <v>7419.7467009305001</v>
       </c>
       <c r="D25" t="s">
@@ -5338,7 +5320,7 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C26" s="21">
         <v>58503.270488649003</v>
       </c>
       <c r="D26" t="s">
@@ -5352,7 +5334,7 @@
       <c r="B27" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="21">
         <v>-17758.112094395001</v>
       </c>
       <c r="D27" t="s">
@@ -5366,7 +5348,7 @@
       <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="21">
         <v>5871.4890342439003</v>
       </c>
       <c r="D28" t="s">
@@ -5380,7 +5362,7 @@
       <c r="B29" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="21">
         <v>11642.939592151</v>
       </c>
       <c r="D29" t="s">
@@ -5394,7 +5376,7 @@
       <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="21">
         <v>20033</v>
       </c>
       <c r="D30" t="s">
@@ -5408,7 +5390,7 @@
       <c r="B31" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="21">
         <v>16524</v>
       </c>
       <c r="D31" t="s">
@@ -5422,7 +5404,7 @@
       <c r="B32" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="21">
         <v>35175</v>
       </c>
       <c r="D32" t="s">
@@ -5436,7 +5418,7 @@
       <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="21">
         <v>37387</v>
       </c>
       <c r="D33" t="s">
@@ -5450,7 +5432,7 @@
       <c r="B34" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="21">
         <v>4419.7323776066996</v>
       </c>
       <c r="D34" t="s">
@@ -5464,7 +5446,7 @@
       <c r="B35" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="21">
         <v>3434.9428690906002</v>
       </c>
       <c r="D35" t="s">
@@ -5478,7 +5460,7 @@
       <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="21">
         <v>4902.2259604786004</v>
       </c>
       <c r="D36" t="s">
@@ -5492,7 +5474,7 @@
       <c r="B37" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="27">
+      <c r="C37" s="21">
         <v>1223.4876227116999</v>
       </c>
       <c r="D37" t="s">
@@ -5506,7 +5488,7 @@
       <c r="B38" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="27">
+      <c r="C38" s="21">
         <v>3740.0275103163999</v>
       </c>
       <c r="D38" t="s">
@@ -5520,7 +5502,7 @@
       <c r="B39" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="27">
+      <c r="C39" s="21">
         <v>-6449.7936726272001</v>
       </c>
       <c r="D39" t="s">
@@ -5534,7 +5516,7 @@
       <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C40" s="21">
         <v>-32731.774415405998</v>
       </c>
       <c r="D40" t="s">
@@ -5548,7 +5530,7 @@
       <c r="B41" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C41" s="21">
         <v>-35738.651994498003</v>
       </c>
       <c r="D41" t="s">
@@ -5562,7 +5544,7 @@
       <c r="B42" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="27">
+      <c r="C42" s="21">
         <v>77569</v>
       </c>
       <c r="D42" t="s">
@@ -5576,7 +5558,7 @@
       <c r="B43" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="27">
+      <c r="C43" s="21">
         <v>77742</v>
       </c>
       <c r="D43" t="s">
@@ -5590,7 +5572,7 @@
       <c r="B44" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="27">
+      <c r="C44" s="21">
         <v>125998</v>
       </c>
       <c r="D44" t="s">
@@ -5604,7 +5586,7 @@
       <c r="B45" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C45" s="21">
         <v>123985</v>
       </c>
       <c r="D45" t="s">
@@ -5618,7 +5600,7 @@
       <c r="B46" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="27">
+      <c r="C46" s="21">
         <v>15115.335985752999</v>
       </c>
       <c r="D46" t="s">
@@ -5632,7 +5614,7 @@
       <c r="B47" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="27">
+      <c r="C47" s="21">
         <v>1153.6039403617999</v>
       </c>
       <c r="D47" t="s">
@@ -5646,7 +5628,7 @@
       <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="27">
+      <c r="C48" s="21">
         <v>4633.2709202634996</v>
       </c>
       <c r="D48" t="s">
@@ -5660,7 +5642,7 @@
       <c r="B49" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="27">
+      <c r="C49" s="21">
         <v>5411.9911166188003</v>
       </c>
       <c r="D49" t="s">
@@ -5674,7 +5656,7 @@
       <c r="B50" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="27">
+      <c r="C50" s="21">
         <v>19162.968441814999</v>
       </c>
       <c r="D50" t="s">
@@ -5688,7 +5670,7 @@
       <c r="B51" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="27">
+      <c r="C51" s="21">
         <v>-607.741617357</v>
       </c>
       <c r="D51" t="s">
@@ -5702,7 +5684,7 @@
       <c r="B52" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="27">
+      <c r="C52" s="21">
         <v>23243.343195265999</v>
       </c>
       <c r="D52" t="s">
@@ -5716,7 +5698,7 @@
       <c r="B53" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="27">
+      <c r="C53" s="21">
         <v>-27703.402366864</v>
       </c>
       <c r="D53" t="s">
@@ -5730,7 +5712,7 @@
       <c r="B54" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="27">
+      <c r="C54" s="21">
         <v>74266</v>
       </c>
       <c r="D54" t="s">
@@ -5744,7 +5726,7 @@
       <c r="B55" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="27">
+      <c r="C55" s="21">
         <v>76247</v>
       </c>
       <c r="D55" t="s">
@@ -5758,7 +5740,7 @@
       <c r="B56" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="27">
+      <c r="C56" s="21">
         <v>98843</v>
       </c>
       <c r="D56" t="s">
@@ -5772,7 +5754,7 @@
       <c r="B57" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="27">
+      <c r="C57" s="21">
         <v>69014</v>
       </c>
       <c r="D57" t="s">
@@ -5786,7 +5768,7 @@
       <c r="B58" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="27">
+      <c r="C58" s="21">
         <v>5724.1095260534003</v>
       </c>
       <c r="D58" t="s">
@@ -5800,7 +5782,7 @@
       <c r="B59" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="27">
+      <c r="C59" s="21">
         <v>2277.4807375427999</v>
       </c>
       <c r="D59" t="s">
@@ -5814,7 +5796,7 @@
       <c r="B60" t="s">
         <v>7</v>
       </c>
-      <c r="C60" s="27">
+      <c r="C60" s="21">
         <v>7427.5503080690996</v>
       </c>
       <c r="D60" t="s">
@@ -5828,7 +5810,7 @@
       <c r="B61" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="27">
+      <c r="C61" s="21">
         <v>12171.940796944</v>
       </c>
       <c r="D61" t="s">
@@ -6242,10 +6224,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05CAB71-902C-472D-ACD6-0ABE0E546B47}">
-  <dimension ref="B1:F4"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6256,71 +6238,163 @@
     <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="25"/>
-      <c r="C1" s="25" t="s">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="25" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="27">
         <v>84.62</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="27">
         <v>125.7</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="27">
         <v>2.8</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="27">
         <v>4.9409999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="27">
         <v>77.28</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="27">
         <v>331.9</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="27">
         <v>3.4</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="27">
         <v>23.32</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="27">
         <v>80.900000000000006</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="27">
         <v>67.3</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="27">
         <v>3.8</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="27">
         <v>3.13</v>
       </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>